<commit_message>
temp_exvel doesnt launch  if no asc file selected
</commit_message>
<xml_diff>
--- a/temp_create_csv.xlsx
+++ b/temp_create_csv.xlsx
@@ -29,6 +29,18 @@
     <t>ELEVATION</t>
   </si>
   <si>
+    <t>STN751</t>
+  </si>
+  <si>
+    <t>286440.7476</t>
+  </si>
+  <si>
+    <t>6215456.2261</t>
+  </si>
+  <si>
+    <t>114.0311</t>
+  </si>
+  <si>
     <t>STNRO</t>
   </si>
   <si>
@@ -65,6 +77,15 @@
     <t>133.2873</t>
   </si>
   <si>
+    <t>MENA</t>
+  </si>
+  <si>
+    <t>291928.7360</t>
+  </si>
+  <si>
+    <t>6221563.0740</t>
+  </si>
+  <si>
     <t>CTL4</t>
   </si>
   <si>
@@ -77,6 +98,18 @@
     <t>125.1082</t>
   </si>
   <si>
+    <t>CTL03</t>
+  </si>
+  <si>
+    <t>286254.9359</t>
+  </si>
+  <si>
+    <t>6215385.8195</t>
+  </si>
+  <si>
+    <t>117.4396</t>
+  </si>
+  <si>
     <t>STN13</t>
   </si>
   <si>
@@ -87,39 +120,6 @@
   </si>
   <si>
     <t>134.7438</t>
-  </si>
-  <si>
-    <t>CTL03</t>
-  </si>
-  <si>
-    <t>286254.9359</t>
-  </si>
-  <si>
-    <t>6215385.8195</t>
-  </si>
-  <si>
-    <t>117.4396</t>
-  </si>
-  <si>
-    <t>MENA</t>
-  </si>
-  <si>
-    <t>291928.7360</t>
-  </si>
-  <si>
-    <t>6221563.0740</t>
-  </si>
-  <si>
-    <t>STN751</t>
-  </si>
-  <si>
-    <t>286440.7476</t>
-  </si>
-  <si>
-    <t>6215456.2261</t>
-  </si>
-  <si>
-    <t>114.0311</t>
   </si>
   <si>
     <t>STN741</t>
@@ -577,35 +577,35 @@
       <c r="C6" t="s">
         <v>22</v>
       </c>
-      <c r="D6" t="s">
-        <v>23</v>
-      </c>
+      <c r="D6" t="s"/>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" t="s">
         <v>24</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>25</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>26</v>
-      </c>
-      <c r="D7" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" t="s">
         <v>28</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>29</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>30</v>
       </c>
-      <c r="D8" t="s"/>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">

</xml_diff>

<commit_message>
sorted the output of the temp_excel file
</commit_message>
<xml_diff>
--- a/temp_create_csv.xlsx
+++ b/temp_create_csv.xlsx
@@ -29,6 +29,99 @@
     <t>ELEVATION</t>
   </si>
   <si>
+    <t>CTL03</t>
+  </si>
+  <si>
+    <t>286254.9359</t>
+  </si>
+  <si>
+    <t>6215385.8195</t>
+  </si>
+  <si>
+    <t>117.4396</t>
+  </si>
+  <si>
+    <t>CTL05</t>
+  </si>
+  <si>
+    <t>287047.0456</t>
+  </si>
+  <si>
+    <t>6215313.2060</t>
+  </si>
+  <si>
+    <t>133.2873</t>
+  </si>
+  <si>
+    <t>CTL4</t>
+  </si>
+  <si>
+    <t>286848.0783</t>
+  </si>
+  <si>
+    <t>6215375.9164</t>
+  </si>
+  <si>
+    <t>125.1082</t>
+  </si>
+  <si>
+    <t>MENA</t>
+  </si>
+  <si>
+    <t>291928.7360</t>
+  </si>
+  <si>
+    <t>6221563.0740</t>
+  </si>
+  <si>
+    <t>STN03</t>
+  </si>
+  <si>
+    <t>285968.9539</t>
+  </si>
+  <si>
+    <t>6215310.3795</t>
+  </si>
+  <si>
+    <t>117.3814</t>
+  </si>
+  <si>
+    <t>STN12</t>
+  </si>
+  <si>
+    <t>287562.1489</t>
+  </si>
+  <si>
+    <t>6215335.6571</t>
+  </si>
+  <si>
+    <t>131.8746</t>
+  </si>
+  <si>
+    <t>STN13</t>
+  </si>
+  <si>
+    <t>287771.7689</t>
+  </si>
+  <si>
+    <t>6215279.6768</t>
+  </si>
+  <si>
+    <t>134.7438</t>
+  </si>
+  <si>
+    <t>STN741</t>
+  </si>
+  <si>
+    <t>287406.6731</t>
+  </si>
+  <si>
+    <t>6215388.5113</t>
+  </si>
+  <si>
+    <t>125.5908</t>
+  </si>
+  <si>
     <t>STN751</t>
   </si>
   <si>
@@ -51,99 +144,6 @@
   </si>
   <si>
     <t>115.5244</t>
-  </si>
-  <si>
-    <t>STN03</t>
-  </si>
-  <si>
-    <t>285968.9539</t>
-  </si>
-  <si>
-    <t>6215310.3795</t>
-  </si>
-  <si>
-    <t>117.3814</t>
-  </si>
-  <si>
-    <t>CTL05</t>
-  </si>
-  <si>
-    <t>287047.0456</t>
-  </si>
-  <si>
-    <t>6215313.2060</t>
-  </si>
-  <si>
-    <t>133.2873</t>
-  </si>
-  <si>
-    <t>MENA</t>
-  </si>
-  <si>
-    <t>291928.7360</t>
-  </si>
-  <si>
-    <t>6221563.0740</t>
-  </si>
-  <si>
-    <t>CTL4</t>
-  </si>
-  <si>
-    <t>286848.0783</t>
-  </si>
-  <si>
-    <t>6215375.9164</t>
-  </si>
-  <si>
-    <t>125.1082</t>
-  </si>
-  <si>
-    <t>CTL03</t>
-  </si>
-  <si>
-    <t>286254.9359</t>
-  </si>
-  <si>
-    <t>6215385.8195</t>
-  </si>
-  <si>
-    <t>117.4396</t>
-  </si>
-  <si>
-    <t>STN13</t>
-  </si>
-  <si>
-    <t>287771.7689</t>
-  </si>
-  <si>
-    <t>6215279.6768</t>
-  </si>
-  <si>
-    <t>134.7438</t>
-  </si>
-  <si>
-    <t>STN741</t>
-  </si>
-  <si>
-    <t>287406.6731</t>
-  </si>
-  <si>
-    <t>6215388.5113</t>
-  </si>
-  <si>
-    <t>125.5908</t>
-  </si>
-  <si>
-    <t>STN12</t>
-  </si>
-  <si>
-    <t>287562.1489</t>
-  </si>
-  <si>
-    <t>6215335.6571</t>
-  </si>
-  <si>
-    <t>131.8746</t>
   </si>
 </sst>
 </file>
@@ -563,21 +563,21 @@
       <c r="C5" t="s">
         <v>18</v>
       </c>
-      <c r="D5" t="s">
-        <v>19</v>
-      </c>
+      <c r="D5" t="s"/>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
         <v>20</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>21</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>22</v>
       </c>
-      <c r="D6" t="s"/>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">

</xml_diff>

<commit_message>
elevation from ASC files <100m are now included
</commit_message>
<xml_diff>
--- a/temp_create_csv.xlsx
+++ b/temp_create_csv.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="24">
   <si>
     <t>POINT</t>
   </si>
@@ -29,121 +29,64 @@
     <t>ELEVATION</t>
   </si>
   <si>
-    <t>CTL03</t>
-  </si>
-  <si>
-    <t>286254.9359</t>
-  </si>
-  <si>
-    <t>6215385.8195</t>
-  </si>
-  <si>
-    <t>117.4396</t>
-  </si>
-  <si>
-    <t>CTL05</t>
-  </si>
-  <si>
-    <t>287047.0456</t>
-  </si>
-  <si>
-    <t>6215313.2060</t>
-  </si>
-  <si>
-    <t>133.2873</t>
-  </si>
-  <si>
-    <t>CTL4</t>
-  </si>
-  <si>
-    <t>286848.0783</t>
-  </si>
-  <si>
-    <t>6215375.9164</t>
-  </si>
-  <si>
-    <t>125.1082</t>
-  </si>
-  <si>
-    <t>MENA</t>
-  </si>
-  <si>
-    <t>291928.7360</t>
-  </si>
-  <si>
-    <t>6221563.0740</t>
-  </si>
-  <si>
-    <t>STN03</t>
-  </si>
-  <si>
-    <t>285968.9539</t>
-  </si>
-  <si>
-    <t>6215310.3795</t>
-  </si>
-  <si>
-    <t>117.3814</t>
-  </si>
-  <si>
-    <t>STN12</t>
-  </si>
-  <si>
-    <t>287562.1489</t>
-  </si>
-  <si>
-    <t>6215335.6571</t>
-  </si>
-  <si>
-    <t>131.8746</t>
-  </si>
-  <si>
-    <t>STN13</t>
-  </si>
-  <si>
-    <t>287771.7689</t>
-  </si>
-  <si>
-    <t>6215279.6768</t>
-  </si>
-  <si>
-    <t>134.7438</t>
-  </si>
-  <si>
-    <t>STN741</t>
-  </si>
-  <si>
-    <t>287406.6731</t>
-  </si>
-  <si>
-    <t>6215388.5113</t>
-  </si>
-  <si>
-    <t>125.5908</t>
-  </si>
-  <si>
-    <t>STN751</t>
-  </si>
-  <si>
-    <t>286440.7476</t>
-  </si>
-  <si>
-    <t>6215456.2261</t>
-  </si>
-  <si>
-    <t>114.0311</t>
-  </si>
-  <si>
-    <t>STNRO</t>
-  </si>
-  <si>
-    <t>285930.9534</t>
-  </si>
-  <si>
-    <t>6215397.8550</t>
-  </si>
-  <si>
-    <t>115.5244</t>
+    <t>6167P</t>
+  </si>
+  <si>
+    <t>289682.9416</t>
+  </si>
+  <si>
+    <t>6190941.7817</t>
+  </si>
+  <si>
+    <t>438.5172</t>
+  </si>
+  <si>
+    <t>CRDX</t>
+  </si>
+  <si>
+    <t>294608.3090</t>
+  </si>
+  <si>
+    <t>6199571.8370</t>
+  </si>
+  <si>
+    <t>380.3520</t>
+  </si>
+  <si>
+    <t>RO</t>
+  </si>
+  <si>
+    <t>289670.8344</t>
+  </si>
+  <si>
+    <t>6192251.0810</t>
+  </si>
+  <si>
+    <t>397.1787</t>
+  </si>
+  <si>
+    <t>STN01</t>
+  </si>
+  <si>
+    <t>289623.4902</t>
+  </si>
+  <si>
+    <t>6192201.6504</t>
+  </si>
+  <si>
+    <t>395.6510</t>
+  </si>
+  <si>
+    <t>SW13</t>
+  </si>
+  <si>
+    <t>289565.8562</t>
+  </si>
+  <si>
+    <t>6192191.0538</t>
+  </si>
+  <si>
+    <t>395.7413</t>
   </si>
 </sst>
 </file>
@@ -483,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -563,90 +506,22 @@
       <c r="C5" t="s">
         <v>18</v>
       </c>
-      <c r="D5" t="s"/>
+      <c r="D5" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" t="s">
         <v>23</v>
-      </c>
-      <c r="B7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" t="s">
-        <v>31</v>
-      </c>
-      <c r="B9" t="s">
-        <v>32</v>
-      </c>
-      <c r="C9" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" t="s">
-        <v>35</v>
-      </c>
-      <c r="B10" t="s">
-        <v>36</v>
-      </c>
-      <c r="C10" t="s">
-        <v>37</v>
-      </c>
-      <c r="D10" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" t="s">
-        <v>39</v>
-      </c>
-      <c r="B11" t="s">
-        <v>40</v>
-      </c>
-      <c r="C11" t="s">
-        <v>41</v>
-      </c>
-      <c r="D11" t="s">
-        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactored GSIFile into own module
</commit_message>
<xml_diff>
--- a/temp_create_csv.xlsx
+++ b/temp_create_csv.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="44">
   <si>
     <t>POINT</t>
   </si>
@@ -29,64 +29,124 @@
     <t>ELEVATION</t>
   </si>
   <si>
-    <t>6167P</t>
-  </si>
-  <si>
-    <t>289682.9416</t>
-  </si>
-  <si>
-    <t>6190941.7817</t>
-  </si>
-  <si>
-    <t>438.5172</t>
-  </si>
-  <si>
-    <t>CRDX</t>
-  </si>
-  <si>
-    <t>294608.3090</t>
-  </si>
-  <si>
-    <t>6199571.8370</t>
-  </si>
-  <si>
-    <t>380.3520</t>
-  </si>
-  <si>
-    <t>RO</t>
-  </si>
-  <si>
-    <t>289670.8344</t>
-  </si>
-  <si>
-    <t>6192251.0810</t>
-  </si>
-  <si>
-    <t>397.1787</t>
-  </si>
-  <si>
-    <t>STN01</t>
-  </si>
-  <si>
-    <t>289623.4902</t>
-  </si>
-  <si>
-    <t>6192201.6504</t>
-  </si>
-  <si>
-    <t>395.6510</t>
-  </si>
-  <si>
-    <t>SW13</t>
-  </si>
-  <si>
-    <t>289565.8562</t>
-  </si>
-  <si>
-    <t>6192191.0538</t>
-  </si>
-  <si>
-    <t>395.7413</t>
+    <t>CTL03</t>
+  </si>
+  <si>
+    <t>286254.9359</t>
+  </si>
+  <si>
+    <t>6215385.8195</t>
+  </si>
+  <si>
+    <t>117.4396</t>
+  </si>
+  <si>
+    <t>CTL05</t>
+  </si>
+  <si>
+    <t>287047.0456</t>
+  </si>
+  <si>
+    <t>6215313.2060</t>
+  </si>
+  <si>
+    <t>133.2873</t>
+  </si>
+  <si>
+    <t>CTL4</t>
+  </si>
+  <si>
+    <t>286848.0783</t>
+  </si>
+  <si>
+    <t>6215375.9164</t>
+  </si>
+  <si>
+    <t>125.1082</t>
+  </si>
+  <si>
+    <t>MENA</t>
+  </si>
+  <si>
+    <t>291928.7360</t>
+  </si>
+  <si>
+    <t>6221563.0740</t>
+  </si>
+  <si>
+    <t>89.1090</t>
+  </si>
+  <si>
+    <t>STN03</t>
+  </si>
+  <si>
+    <t>285968.9539</t>
+  </si>
+  <si>
+    <t>6215310.3795</t>
+  </si>
+  <si>
+    <t>117.3814</t>
+  </si>
+  <si>
+    <t>STN12</t>
+  </si>
+  <si>
+    <t>287562.1489</t>
+  </si>
+  <si>
+    <t>6215335.6571</t>
+  </si>
+  <si>
+    <t>131.8746</t>
+  </si>
+  <si>
+    <t>STN13</t>
+  </si>
+  <si>
+    <t>287771.7689</t>
+  </si>
+  <si>
+    <t>6215279.6768</t>
+  </si>
+  <si>
+    <t>134.7438</t>
+  </si>
+  <si>
+    <t>STN741</t>
+  </si>
+  <si>
+    <t>287406.6731</t>
+  </si>
+  <si>
+    <t>6215388.5113</t>
+  </si>
+  <si>
+    <t>125.5908</t>
+  </si>
+  <si>
+    <t>STN751</t>
+  </si>
+  <si>
+    <t>286440.7476</t>
+  </si>
+  <si>
+    <t>6215456.2261</t>
+  </si>
+  <si>
+    <t>114.0311</t>
+  </si>
+  <si>
+    <t>STNRO</t>
+  </si>
+  <si>
+    <t>285930.9534</t>
+  </si>
+  <si>
+    <t>6215397.8550</t>
+  </si>
+  <si>
+    <t>115.5244</t>
   </si>
 </sst>
 </file>
@@ -426,7 +486,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -524,6 +584,76 @@
         <v>23</v>
       </c>
     </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" t="s">
+        <v>43</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>